<commit_message>
Basis für Weiterentwicklung durch HTBL
</commit_message>
<xml_diff>
--- a/__Doku/00 Datenstruktur LightLife.xlsx
+++ b/__Doku/00 Datenstruktur LightLife.xlsx
@@ -4224,7 +4224,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4339,8 +4339,8 @@
       <c r="B9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>113</v>
+      <c r="C9" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="D9" s="2"/>
     </row>

</xml_diff>